<commit_message>
Added application security key to the getubmpagereference.php json request.
A UBM Application key must be used to authenticate the application with
all requests to this resource.
</commit_message>
<xml_diff>
--- a/Documentation/Website Documentation Template/RDBMS Hierarchical Objects Schema.xlsx
+++ b/Documentation/Website Documentation Template/RDBMS Hierarchical Objects Schema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="28720" yWindow="0" windowWidth="20480" windowHeight="14920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Path Enumeration" sheetId="1" r:id="rId1"/>
@@ -728,10 +728,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -760,9 +762,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -780,8 +779,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -794,6 +796,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -806,6 +809,7 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -1178,7 +1182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1370,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1538,14 +1542,14 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="21"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
@@ -1627,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1733,19 +1737,19 @@
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>81</v>
       </c>
       <c r="I19" s="2" t="s">
@@ -1753,19 +1757,19 @@
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="8">
-        <v>1</v>
-      </c>
-      <c r="B20" s="9" t="s">
+      <c r="A20" s="7">
+        <v>1</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="8">
-        <v>1</v>
-      </c>
-      <c r="G20" s="21">
+      <c r="F20" s="7">
+        <v>1</v>
+      </c>
+      <c r="G20" s="20">
         <v>1</v>
       </c>
       <c r="J20" s="3" t="s">
@@ -1773,192 +1777,192 @@
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="8">
+      <c r="A21" s="7">
         <v>2</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="8">
-        <v>1</v>
-      </c>
-      <c r="G21" s="21">
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+      <c r="G21" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="8">
+      <c r="A22" s="7">
         <v>3</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="8">
-        <v>1</v>
-      </c>
-      <c r="G22" s="21">
+      <c r="F22" s="7">
+        <v>1</v>
+      </c>
+      <c r="G22" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="8">
+      <c r="A23" s="7">
         <v>4</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="8">
-        <v>1</v>
-      </c>
-      <c r="G23" s="21">
+      <c r="F23" s="7">
+        <v>1</v>
+      </c>
+      <c r="G23" s="20">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="8">
+      <c r="A24" s="7">
         <v>5</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="8">
-        <v>1</v>
-      </c>
-      <c r="G24" s="21">
+      <c r="F24" s="7">
+        <v>1</v>
+      </c>
+      <c r="G24" s="20">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="8">
+      <c r="A25" s="7">
         <v>6</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="8">
-        <v>1</v>
-      </c>
-      <c r="G25" s="21">
+      <c r="F25" s="7">
+        <v>1</v>
+      </c>
+      <c r="G25" s="20">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="16" thickBot="1">
-      <c r="A26" s="11">
+      <c r="A26" s="10">
         <v>7</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F26" s="8">
-        <v>1</v>
-      </c>
-      <c r="G26" s="21">
+      <c r="F26" s="7">
+        <v>1</v>
+      </c>
+      <c r="G26" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="F27" s="8">
+      <c r="F27" s="7">
         <v>2</v>
       </c>
-      <c r="G27" s="10">
+      <c r="G27" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="F28" s="8">
+      <c r="F28" s="7">
         <v>2</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="F29" s="8">
+      <c r="F29" s="7">
         <v>3</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="F30" s="8">
+      <c r="F30" s="7">
         <v>4</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G30" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="F31" s="8">
+      <c r="F31" s="7">
         <v>4</v>
       </c>
-      <c r="G31" s="10">
+      <c r="G31" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="F32" s="8">
+      <c r="F32" s="7">
         <v>4</v>
       </c>
-      <c r="G32" s="10">
+      <c r="G32" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="F33" s="8">
+      <c r="F33" s="7">
         <v>4</v>
       </c>
-      <c r="G33" s="10">
+      <c r="G33" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="F34" s="8">
+      <c r="F34" s="7">
         <v>5</v>
       </c>
-      <c r="G34" s="10">
+      <c r="G34" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="F35" s="8">
+      <c r="F35" s="7">
         <v>6</v>
       </c>
-      <c r="G35" s="10">
+      <c r="G35" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="F36" s="8">
+      <c r="F36" s="7">
         <v>6</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G36" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="16" thickBot="1">
-      <c r="F37" s="11">
+      <c r="F37" s="10">
         <v>7</v>
       </c>
-      <c r="G37" s="13">
+      <c r="G37" s="12">
         <v>7</v>
       </c>
     </row>
@@ -1971,430 +1975,428 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="F41" s="5" t="s">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="G41" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H41" s="7" t="s">
+      <c r="H41" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" t="s">
-        <v>84</v>
-      </c>
-      <c r="F42" s="8">
-        <v>1</v>
-      </c>
-      <c r="G42" s="9">
-        <v>1</v>
-      </c>
-      <c r="H42" s="10">
+      <c r="B42" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1</v>
+      </c>
+      <c r="G42" s="8">
+        <v>1</v>
+      </c>
+      <c r="H42" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="B43" t="s">
-        <v>85</v>
-      </c>
-      <c r="F43" s="8">
-        <v>1</v>
-      </c>
-      <c r="G43" s="9">
+        <v>86</v>
+      </c>
+      <c r="F43" s="7">
+        <v>1</v>
+      </c>
+      <c r="G43" s="8">
         <v>2</v>
       </c>
-      <c r="H43" s="10">
+      <c r="H43" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="B44" t="s">
-        <v>86</v>
-      </c>
-      <c r="F44" s="8">
-        <v>1</v>
-      </c>
-      <c r="G44" s="9">
+      <c r="F44" s="7">
+        <v>1</v>
+      </c>
+      <c r="G44" s="8">
         <v>3</v>
       </c>
-      <c r="H44" s="10">
+      <c r="H44" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="F45" s="8">
-        <v>1</v>
-      </c>
-      <c r="G45" s="9">
+      <c r="F45" s="7">
+        <v>1</v>
+      </c>
+      <c r="G45" s="8">
         <v>4</v>
       </c>
-      <c r="H45" s="10">
+      <c r="H45" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="F46" s="8">
-        <v>1</v>
-      </c>
-      <c r="G46" s="9">
+      <c r="A46" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46" s="7">
+        <v>1</v>
+      </c>
+      <c r="G46" s="8">
         <v>5</v>
       </c>
-      <c r="H46" s="10">
+      <c r="H46" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F47" s="8">
-        <v>1</v>
-      </c>
-      <c r="G47" s="9">
+      <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="F47" s="7">
+        <v>1</v>
+      </c>
+      <c r="G47" s="8">
         <v>6</v>
       </c>
-      <c r="H47" s="10">
+      <c r="H47" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" t="s">
-        <v>92</v>
-      </c>
-      <c r="F48" s="8">
-        <v>1</v>
-      </c>
-      <c r="G48" s="9">
+      <c r="B48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F48" s="7">
+        <v>1</v>
+      </c>
+      <c r="G48" s="8">
         <v>7</v>
       </c>
-      <c r="H48" s="10">
+      <c r="H48" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="B49" t="s">
-        <v>88</v>
-      </c>
-      <c r="F49" s="8">
+        <v>89</v>
+      </c>
+      <c r="F49" s="7">
         <v>2</v>
       </c>
-      <c r="G49" s="9">
+      <c r="G49" s="8">
         <v>2</v>
       </c>
-      <c r="H49" s="10">
+      <c r="H49" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="B50" t="s">
-        <v>89</v>
-      </c>
-      <c r="F50" s="8">
+        <v>90</v>
+      </c>
+      <c r="F50" s="7">
         <v>2</v>
       </c>
-      <c r="G50" s="9">
+      <c r="G50" s="8">
         <v>3</v>
       </c>
-      <c r="H50" s="10">
+      <c r="H50" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="B51" t="s">
-        <v>90</v>
-      </c>
-      <c r="F51" s="8">
+      <c r="F51" s="7">
         <v>3</v>
       </c>
-      <c r="G51" s="9">
+      <c r="G51" s="8">
         <v>3</v>
       </c>
-      <c r="H51" s="10">
+      <c r="H51" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="F52" s="8">
+      <c r="A52" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F52" s="7">
         <v>4</v>
       </c>
-      <c r="G52" s="9">
+      <c r="G52" s="8">
         <v>4</v>
       </c>
-      <c r="H52" s="10">
+      <c r="H52" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F53" s="8">
+      <c r="A53" t="s">
+        <v>93</v>
+      </c>
+      <c r="F53" s="7">
         <v>4</v>
       </c>
-      <c r="G53" s="9">
+      <c r="G53" s="8">
         <v>5</v>
       </c>
-      <c r="H53" s="10">
+      <c r="H53" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>93</v>
-      </c>
-      <c r="F54" s="8">
+        <v>94</v>
+      </c>
+      <c r="F54" s="7">
         <v>4</v>
       </c>
-      <c r="G54" s="9">
+      <c r="G54" s="8">
         <v>6</v>
       </c>
-      <c r="H54" s="10">
+      <c r="H54" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" t="s">
-        <v>94</v>
-      </c>
-      <c r="F55" s="8">
+      <c r="B55" t="s">
+        <v>95</v>
+      </c>
+      <c r="F55" s="7">
         <v>4</v>
       </c>
-      <c r="G55" s="9">
+      <c r="G55" s="8">
         <v>7</v>
       </c>
-      <c r="H55" s="10">
+      <c r="H55" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="B56" t="s">
-        <v>95</v>
-      </c>
-      <c r="F56" s="8">
+        <v>96</v>
+      </c>
+      <c r="F56" s="7">
         <v>5</v>
       </c>
-      <c r="G56" s="9">
+      <c r="G56" s="8">
         <v>5</v>
       </c>
-      <c r="H56" s="10">
+      <c r="H56" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="B57" t="s">
-        <v>96</v>
-      </c>
-      <c r="F57" s="8">
+        <v>97</v>
+      </c>
+      <c r="F57" s="7">
         <v>6</v>
       </c>
-      <c r="G57" s="9">
+      <c r="G57" s="8">
         <v>6</v>
       </c>
-      <c r="H57" s="10">
+      <c r="H57" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="B58" t="s">
-        <v>97</v>
-      </c>
-      <c r="F58" s="8">
+      <c r="F58" s="7">
         <v>6</v>
       </c>
-      <c r="G58" s="9">
+      <c r="G58" s="8">
         <v>7</v>
       </c>
-      <c r="H58" s="10">
+      <c r="H58" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="16" thickBot="1">
-      <c r="F59" s="11">
+      <c r="A59" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F59" s="10">
         <v>7</v>
       </c>
-      <c r="G59" s="12">
+      <c r="G59" s="11">
         <v>7</v>
       </c>
-      <c r="H59" s="13">
+      <c r="H59" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="2" t="s">
-        <v>98</v>
+      <c r="A60" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="B62" t="s">
+      <c r="B61" t="s">
         <v>100</v>
       </c>
     </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="2" t="s">
-        <v>101</v>
+      <c r="A64" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" t="s">
-        <v>102</v>
+      <c r="B65" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="B66" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
-      <c r="B67" t="s">
         <v>104</v>
       </c>
     </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="70" spans="1:10">
-      <c r="A70" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="A71" t="s">
+      <c r="A70" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="16" thickBot="1"/>
     <row r="74" spans="1:10">
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C74" s="15" t="s">
+      <c r="C74" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D74" s="15" t="s">
+      <c r="D74" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="E74" s="15" t="s">
+      <c r="E74" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="F74" s="15" t="s">
+      <c r="F74" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="G74" s="15" t="s">
+      <c r="G74" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="H74" s="15" t="s">
+      <c r="H74" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="I74" s="16" t="s">
+      <c r="I74" s="15" t="s">
         <v>116</v>
       </c>
       <c r="J74" s="2"/>
     </row>
     <row r="75" spans="1:10">
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C75" s="9">
-        <v>1</v>
-      </c>
-      <c r="D75" s="9" t="s">
+      <c r="C75" s="8">
+        <v>1</v>
+      </c>
+      <c r="D75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E75" s="17" t="s">
+      <c r="E75" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="F75" s="9" t="s">
+      <c r="F75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G75" s="9" t="s">
+      <c r="G75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H75" s="9" t="s">
+      <c r="H75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="I75" s="10" t="s">
+      <c r="I75" s="9" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:10">
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C76" s="9">
-        <v>1</v>
-      </c>
-      <c r="D76" s="9" t="s">
+      <c r="C76" s="8">
+        <v>1</v>
+      </c>
+      <c r="D76" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="E76" s="9" t="s">
+      <c r="E76" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="F76" s="9" t="s">
+      <c r="F76" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G76" s="9" t="s">
+      <c r="G76" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H76" s="9" t="s">
+      <c r="H76" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="I76" s="10" t="s">
+      <c r="I76" s="9" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:10">
-      <c r="B77" s="8" t="s">
+      <c r="B77" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C77" s="9">
-        <v>1</v>
-      </c>
-      <c r="D77" s="9" t="s">
+      <c r="C77" s="8">
+        <v>1</v>
+      </c>
+      <c r="D77" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="E77" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="F77" s="17" t="s">
+      <c r="F77" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="G77" s="17" t="s">
+      <c r="G77" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="H77" s="17" t="s">
+      <c r="H77" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="I77" s="18" t="s">
+      <c r="I77" s="17" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="16" thickBot="1">
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C78" s="12">
+      <c r="C78" s="11">
         <v>2</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D78" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E78" s="12" t="s">
+      <c r="E78" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="F78" s="12" t="s">
+      <c r="F78" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="G78" s="12" t="s">
+      <c r="G78" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="H78" s="12" t="s">
+      <c r="H78" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="I78" s="13" t="s">
+      <c r="I78" s="12" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2430,7 +2432,7 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2799,22 +2801,22 @@
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="D62" s="19" t="s">
+      <c r="D62" s="18" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="E63" s="19" t="s">
+      <c r="E63" s="18" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="D64" s="20" t="s">
+      <c r="D64" s="19" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="65" spans="5:5">
-      <c r="E65" s="20" t="s">
+      <c r="E65" s="19" t="s">
         <v>172</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added UBMS functionality to ubmpageref requests.
Added UBMS functionality to ubmpageref requests.
</commit_message>
<xml_diff>
--- a/Documentation/Website Documentation Template/RDBMS Hierarchical Objects Schema.xlsx
+++ b/Documentation/Website Documentation Template/RDBMS Hierarchical Objects Schema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28720" yWindow="0" windowWidth="20480" windowHeight="14920" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-25520" yWindow="0" windowWidth="25520" windowHeight="20040" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Path Enumeration" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="187">
   <si>
     <t>Path Enumeration</t>
   </si>
@@ -547,6 +547,42 @@
   </si>
   <si>
     <t>(Using SQL-99 recursive) BAD IF USING</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>JD</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>Get ActiveModel</t>
+  </si>
+  <si>
+    <t>Get All Possible (reference manual)</t>
   </si>
 </sst>
 </file>
@@ -615,7 +651,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -635,6 +671,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,7 +770,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -756,8 +798,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -782,8 +830,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="33">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -797,6 +857,9 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -810,6 +873,9 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -1629,10 +1695,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q78"/>
+  <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1926,7 +1992,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:23">
       <c r="F33" s="7">
         <v>4</v>
       </c>
@@ -1934,7 +2000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:23">
       <c r="F34" s="7">
         <v>5</v>
       </c>
@@ -1942,39 +2008,247 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:23" ht="30" customHeight="1">
       <c r="F35" s="7">
         <v>6</v>
       </c>
       <c r="G35" s="9">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="L35" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="S35" s="22"/>
+      <c r="T35" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="U35" s="27"/>
+      <c r="V35" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="W35" s="26"/>
+    </row>
+    <row r="36" spans="1:23">
       <c r="F36" s="7">
         <v>6</v>
       </c>
       <c r="G36" s="9">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="16" thickBot="1">
+      <c r="L36" t="s">
+        <v>175</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36" t="s">
+        <v>175</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="R36" t="s">
+        <v>175</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+      <c r="T36" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="U36" s="25">
+        <v>1</v>
+      </c>
+      <c r="V36" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="W36" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="16" thickBot="1">
       <c r="F37" s="10">
         <v>7</v>
       </c>
       <c r="G37" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="16" thickBot="1">
+      <c r="L37" t="s">
+        <v>176</v>
+      </c>
+      <c r="M37">
+        <v>2</v>
+      </c>
+      <c r="N37" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="O37" s="23">
+        <v>2</v>
+      </c>
+      <c r="P37" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q37">
+        <v>2</v>
+      </c>
+      <c r="R37" t="s">
+        <v>176</v>
+      </c>
+      <c r="S37">
+        <v>2</v>
+      </c>
+      <c r="T37" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="U37" s="25">
+        <v>2</v>
+      </c>
+      <c r="V37" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="W37" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23">
+      <c r="L38" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="M38" s="23">
+        <v>3</v>
+      </c>
+      <c r="N38" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="O38" s="23">
+        <v>3</v>
+      </c>
+      <c r="P38" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q38">
+        <v>3</v>
+      </c>
+      <c r="R38" t="s">
+        <v>179</v>
+      </c>
+      <c r="S38">
+        <v>3</v>
+      </c>
+      <c r="T38" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="U38" s="25">
+        <v>3</v>
+      </c>
+      <c r="V38" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="W38" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23">
+      <c r="L39" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="M39" s="23">
+        <v>4</v>
+      </c>
+      <c r="N39" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="O39" s="23">
+        <v>4</v>
+      </c>
+      <c r="P39" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q39">
+        <v>4</v>
+      </c>
+      <c r="R39" t="s">
+        <v>177</v>
+      </c>
+      <c r="S39">
+        <v>4</v>
+      </c>
+      <c r="T39" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="U39" s="25">
+        <v>4</v>
+      </c>
+      <c r="V39" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="W39" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="16" thickBot="1">
       <c r="A40" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="L40" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="M40" s="23">
+        <v>5</v>
+      </c>
+      <c r="N40" t="s">
+        <v>178</v>
+      </c>
+      <c r="O40">
+        <v>5</v>
+      </c>
+      <c r="P40" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q40">
+        <v>5</v>
+      </c>
+      <c r="R40" t="s">
+        <v>178</v>
+      </c>
+      <c r="S40">
+        <v>5</v>
+      </c>
+      <c r="T40" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="U40" s="25">
+        <v>5</v>
+      </c>
+      <c r="V40" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="W40" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -1987,8 +2261,44 @@
       <c r="H41" s="6" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="L41" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="M41" s="23">
+        <v>6</v>
+      </c>
+      <c r="N41" t="s">
+        <v>180</v>
+      </c>
+      <c r="O41">
+        <v>6</v>
+      </c>
+      <c r="P41" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q41">
+        <v>6</v>
+      </c>
+      <c r="R41" t="s">
+        <v>180</v>
+      </c>
+      <c r="S41">
+        <v>6</v>
+      </c>
+      <c r="T41" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="U41" s="25">
+        <v>6</v>
+      </c>
+      <c r="V41" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="W41" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23">
       <c r="B42" t="s">
         <v>85</v>
       </c>
@@ -2001,72 +2311,108 @@
       <c r="H42" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="L42" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="M42" s="23">
+        <v>7</v>
+      </c>
+      <c r="N42" t="s">
+        <v>181</v>
+      </c>
+      <c r="O42">
+        <v>7</v>
+      </c>
+      <c r="P42" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q42">
+        <v>7</v>
+      </c>
+      <c r="R42" t="s">
+        <v>181</v>
+      </c>
+      <c r="S42">
+        <v>7</v>
+      </c>
+      <c r="T42" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="U42" s="25">
+        <v>7</v>
+      </c>
+      <c r="V42" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="W42" s="25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23">
       <c r="B43" t="s">
         <v>86</v>
       </c>
       <c r="F43" s="7">
         <v>1</v>
       </c>
-      <c r="G43" s="8">
+      <c r="G43" s="24">
         <v>2</v>
       </c>
       <c r="H43" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:23">
       <c r="F44" s="7">
         <v>1</v>
       </c>
-      <c r="G44" s="8">
+      <c r="G44" s="24">
         <v>3</v>
       </c>
       <c r="H44" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:23">
       <c r="F45" s="7">
         <v>1</v>
       </c>
-      <c r="G45" s="8">
+      <c r="G45" s="24">
         <v>4</v>
       </c>
       <c r="H45" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:23">
       <c r="A46" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F46" s="7">
         <v>1</v>
       </c>
-      <c r="G46" s="8">
+      <c r="G46" s="24">
         <v>5</v>
       </c>
       <c r="H46" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:23">
       <c r="A47" t="s">
         <v>92</v>
       </c>
       <c r="F47" s="7">
         <v>1</v>
       </c>
-      <c r="G47" s="8">
+      <c r="G47" s="24">
         <v>6</v>
       </c>
       <c r="H47" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:23">
       <c r="B48" t="s">
         <v>88</v>
       </c>
@@ -2401,6 +2747,14 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="R35:S35"/>
+    <mergeCell ref="T35:U35"/>
+    <mergeCell ref="V35:W35"/>
+  </mergeCells>
   <conditionalFormatting sqref="D75:H78">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",D75)))</formula>

</xml_diff>

<commit_message>
Modified the Application Key to be set in a single place to increase security. Added functionality to the getMyModelsListofApplications() function.
A dashboard/placeholder page is inserted on load for each application
that has been added to the model.
</commit_message>
<xml_diff>
--- a/Documentation/Website Documentation Template/RDBMS Hierarchical Objects Schema.xlsx
+++ b/Documentation/Website Documentation Template/RDBMS Hierarchical Objects Schema.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="188">
   <si>
     <t>Path Enumeration</t>
   </si>
@@ -579,10 +579,13 @@
     <t>Remove</t>
   </si>
   <si>
-    <t>Get ActiveModel</t>
-  </si>
-  <si>
     <t>Get All Possible (reference manual)</t>
+  </si>
+  <si>
+    <t>Get Current Model</t>
+  </si>
+  <si>
+    <t>Publish MFI</t>
   </si>
 </sst>
 </file>
@@ -1697,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N47" sqref="N47"/>
+    <sheetView tabSelected="1" topLeftCell="G12" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37:Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2028,15 +2031,15 @@
       </c>
       <c r="Q35" s="22"/>
       <c r="R35" s="22" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="S35" s="22"/>
       <c r="T35" s="27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U35" s="27"/>
       <c r="V35" s="26" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="W35" s="26"/>
     </row>
@@ -2217,10 +2220,10 @@
       <c r="M40" s="23">
         <v>5</v>
       </c>
-      <c r="N40" t="s">
+      <c r="N40" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="O40">
+      <c r="O40" s="23">
         <v>5</v>
       </c>
       <c r="P40" t="s">
@@ -2267,10 +2270,10 @@
       <c r="M41" s="23">
         <v>6</v>
       </c>
-      <c r="N41" t="s">
+      <c r="N41" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="O41">
+      <c r="O41" s="23">
         <v>6</v>
       </c>
       <c r="P41" t="s">
@@ -2317,10 +2320,10 @@
       <c r="M42" s="23">
         <v>7</v>
       </c>
-      <c r="N42" t="s">
+      <c r="N42" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="O42">
+      <c r="O42" s="23">
         <v>7</v>
       </c>
       <c r="P42" t="s">

</xml_diff>